<commit_message>
migraciones countries companies clubs
</commit_message>
<xml_diff>
--- a/BBDD.xlsx
+++ b/BBDD.xlsx
@@ -82,9 +82,6 @@
     <t>company_id</t>
   </si>
   <si>
-    <t>company</t>
-  </si>
-  <si>
     <t>legal_form</t>
   </si>
   <si>
@@ -299,13 +296,16 @@
   </si>
   <si>
     <t>obsrvations</t>
+  </si>
+  <si>
+    <t>companies</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -359,6 +359,14 @@
       <u/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -448,7 +456,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -482,6 +490,7 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -550,9 +559,9 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>866775</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>981075</xdr:colOff>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:to>
@@ -568,8 +577,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3124200" y="1800225"/>
-          <a:ext cx="847725" cy="790575"/>
+          <a:off x="1590675" y="1990725"/>
+          <a:ext cx="2381250" cy="600075"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -1781,7 +1790,7 @@
   <dimension ref="B1:Q49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1804,20 +1813,20 @@
       <c r="H1" s="2"/>
     </row>
     <row r="2" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H2" s="23" t="s">
         <v>10</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="2:17" x14ac:dyDescent="0.25">
@@ -1828,7 +1837,7 @@
         <v>0</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H3" s="3" t="s">
         <v>0</v>
@@ -1871,7 +1880,7 @@
         <v>18</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="L5" s="2" t="s">
         <v>1</v>
@@ -1897,7 +1906,7 @@
         <v>2</v>
       </c>
       <c r="Q6" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="2:17" x14ac:dyDescent="0.25">
@@ -1911,10 +1920,10 @@
         <v>13</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="Q7" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="2:17" x14ac:dyDescent="0.25">
@@ -1922,35 +1931,35 @@
         <v>3</v>
       </c>
       <c r="F8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H8" s="2" t="s">
         <v>15</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="Q8" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="9" spans="2:17" x14ac:dyDescent="0.25">
       <c r="D9" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H9" s="2" t="s">
         <v>16</v>
       </c>
       <c r="Q9" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="10" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B10" s="1" t="s">
-        <v>22</v>
+      <c r="B10" s="23" t="s">
+        <v>94</v>
       </c>
       <c r="D10" s="8" t="s">
         <v>21</v>
@@ -1959,7 +1968,7 @@
         <v>17</v>
       </c>
       <c r="Q10" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11" spans="2:17" x14ac:dyDescent="0.25">
@@ -1970,15 +1979,15 @@
         <v>7</v>
       </c>
       <c r="Q11" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="12" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="Q12" s="2" t="s">
         <v>12</v>
@@ -1986,22 +1995,22 @@
     </row>
     <row r="13" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F13" s="8" t="s">
         <v>19</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I13" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="K13" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="K13" s="5" t="s">
-        <v>34</v>
-      </c>
       <c r="N13" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="Q13" s="2" t="s">
         <v>13</v>
@@ -2038,10 +2047,10 @@
         <v>1</v>
       </c>
       <c r="K15" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="N15" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="Q15" s="2" t="s">
         <v>14</v>
@@ -2061,10 +2070,10 @@
         <v>19</v>
       </c>
       <c r="N16" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="Q16" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="17" spans="2:17" x14ac:dyDescent="0.25">
@@ -2072,7 +2081,7 @@
         <v>14</v>
       </c>
       <c r="F17" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I17" s="2" t="s">
         <v>20</v>
@@ -2082,7 +2091,7 @@
         <v>20</v>
       </c>
       <c r="Q17" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="18" spans="2:17" x14ac:dyDescent="0.25">
@@ -2107,18 +2116,18 @@
     </row>
     <row r="20" spans="2:17" x14ac:dyDescent="0.25">
       <c r="E20" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H20" s="17"/>
       <c r="I20" s="18"/>
       <c r="N20" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Q20" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="21" spans="2:17" x14ac:dyDescent="0.25">
@@ -2128,20 +2137,20 @@
       <c r="H21" s="19"/>
       <c r="I21" s="19"/>
       <c r="N21" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="Q21" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="22" spans="2:17" x14ac:dyDescent="0.25">
       <c r="F22" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H22" s="19"/>
       <c r="I22" s="19"/>
       <c r="N22" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="23" spans="2:17" x14ac:dyDescent="0.25">
@@ -2151,17 +2160,18 @@
       <c r="H23" s="19"/>
       <c r="I23" s="19"/>
       <c r="N23" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="24" spans="2:17" x14ac:dyDescent="0.25">
       <c r="F24" s="2" t="s">
         <v>20</v>
       </c>
+      <c r="G24" s="15"/>
       <c r="H24" s="19"/>
       <c r="I24" s="19"/>
       <c r="N24" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="25" spans="2:17" x14ac:dyDescent="0.25">
@@ -2176,10 +2186,10 @@
       <c r="H27" s="16"/>
       <c r="I27" s="16"/>
       <c r="K27" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="N27" s="1" t="s">
         <v>78</v>
-      </c>
-      <c r="N27" s="1" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="28" spans="2:17" x14ac:dyDescent="0.25">
@@ -2192,22 +2202,22 @@
     </row>
     <row r="29" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B29" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F29" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G29" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K29" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="N29" s="8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="30" spans="2:17" x14ac:dyDescent="0.25">
@@ -2225,52 +2235,52 @@
         <v>1</v>
       </c>
       <c r="G31" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K31" s="20" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="N31" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="32" spans="2:17" x14ac:dyDescent="0.25">
       <c r="C32" s="2"/>
       <c r="F32" s="15"/>
       <c r="G32" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H32" s="14" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K32" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="N32" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="33" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C33" s="2"/>
       <c r="G33" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="H33" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="H33" s="14" t="s">
-        <v>66</v>
-      </c>
       <c r="K33" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="N33" s="21" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="34" spans="2:14" x14ac:dyDescent="0.25">
       <c r="G34" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H34" s="14" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="N34" s="2" t="s">
         <v>20</v>
@@ -2278,33 +2288,33 @@
     </row>
     <row r="35" spans="2:14" x14ac:dyDescent="0.25">
       <c r="G35" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H35" s="14" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J35" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K35" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="36" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B36" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G36" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H36" s="14" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K36" s="3" t="s">
         <v>0</v>
       </c>
       <c r="N36" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="37" spans="2:14" x14ac:dyDescent="0.25">
@@ -2312,10 +2322,10 @@
         <v>0</v>
       </c>
       <c r="G37" s="12" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H37" s="14" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="K37" s="2" t="s">
         <v>1</v>
@@ -2326,18 +2336,18 @@
     </row>
     <row r="38" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B38" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K38" s="2" t="s">
         <v>11</v>
       </c>
       <c r="N38" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="39" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B39" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K39" s="2" t="s">
         <v>20</v>
@@ -2348,13 +2358,13 @@
     </row>
     <row r="40" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B40" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K40" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="N40" s="8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="41" spans="2:14" x14ac:dyDescent="0.25">
@@ -2362,10 +2372,10 @@
         <v>11</v>
       </c>
       <c r="K41" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="N41" s="8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="42" spans="2:14" x14ac:dyDescent="0.25">
@@ -2389,7 +2399,7 @@
         <v>15</v>
       </c>
       <c r="J45" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="46" spans="2:14" x14ac:dyDescent="0.25">
@@ -2402,12 +2412,12 @@
     </row>
     <row r="47" spans="2:14" x14ac:dyDescent="0.25">
       <c r="J47" s="8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="48" spans="2:14" x14ac:dyDescent="0.25">
       <c r="J48" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="49" spans="10:10" x14ac:dyDescent="0.25">

</xml_diff>